<commit_message>
TrapezeWorkloadPartitioner with trapeze area
Cf. https://github.com/gfoidl/Stochastics/pull/11#discussion_r159157341
</commit_message>
<xml_diff>
--- a/source/gfoidl.Stochastics/Partitioners/Calcs.xlsx
+++ b/source/gfoidl.Stochastics/Partitioners/Calcs.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Triangle" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Trapeze" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
   <si>
-    <t>n</t>
+    <t>N </t>
   </si>
   <si>
-    <t>n2</t>
+    <t>N2</t>
   </si>
   <si>
     <t>lambda</t>
@@ -66,6 +67,21 @@
   <si>
     <t>Sum Delta</t>
   </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>A </t>
+  </si>
+  <si>
+    <t>A/lambda</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Area exact</t>
+  </si>
 </sst>
 </file>
 
@@ -76,11 +92,12 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,19 +119,30 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +165,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9999"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF66"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -174,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,15 +225,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,6 +278,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,7 +334,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFCCFF66"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF9999"/>
@@ -319,7 +361,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart91.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -331,7 +373,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -344,7 +386,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" spc="-1" strike="noStrike">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -371,7 +413,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Triangle!$F$8</c:f>
+              <c:f>Triangle!$F$8:$F$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -395,6 +437,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -447,8 +490,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="98768199"/>
-        <c:axId val="2349983"/>
+        <c:axId val="71436269"/>
+        <c:axId val="70410611"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -457,7 +500,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Triangle!$G$8</c:f>
+              <c:f>Triangle!$G$8:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -481,6 +524,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -533,11 +577,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="99072555"/>
-        <c:axId val="60218254"/>
+        <c:axId val="44846567"/>
+        <c:axId val="53326331"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98768199"/>
+        <c:axId val="71436269"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,7 +594,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -563,7 +607,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -610,14 +654,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2349983"/>
+        <c:crossAx val="70410611"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2349983"/>
+        <c:axId val="70410611"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,7 +683,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -652,7 +696,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -670,7 +714,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -699,11 +743,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98768199"/>
+        <c:crossAx val="71436269"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="99072555"/>
+        <c:axId val="44846567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,7 +760,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -729,7 +773,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -776,14 +820,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60218254"/>
+        <c:crossAx val="53326331"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60218254"/>
+        <c:axId val="53326331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,7 +840,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -809,7 +853,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -827,7 +871,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -856,7 +900,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99072555"/>
+        <c:crossAx val="44846567"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -882,7 +926,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart92.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -894,7 +938,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -907,7 +951,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" spc="-1" strike="noStrike">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -958,6 +1002,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1010,8 +1055,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="85040092"/>
-        <c:axId val="18424344"/>
+        <c:axId val="81619490"/>
+        <c:axId val="83193813"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1044,6 +1089,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1096,11 +1142,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="81731031"/>
-        <c:axId val="92733178"/>
+        <c:axId val="50071952"/>
+        <c:axId val="29861765"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85040092"/>
+        <c:axId val="81619490"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1159,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1126,7 +1172,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1173,14 +1219,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18424344"/>
+        <c:crossAx val="83193813"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18424344"/>
+        <c:axId val="83193813"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,7 +1248,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1215,7 +1261,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1233,7 +1279,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1262,11 +1308,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85040092"/>
+        <c:crossAx val="81619490"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="81731031"/>
+        <c:axId val="50071952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,7 +1325,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1292,7 +1338,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1339,14 +1385,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92733178"/>
+        <c:crossAx val="29861765"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92733178"/>
+        <c:axId val="29861765"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,7 +1405,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1372,7 +1418,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1390,7 +1436,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1419,7 +1465,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81731031"/>
+        <c:crossAx val="50071952"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -1445,7 +1491,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart93.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1457,7 +1503,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1470,7 +1516,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" spc="-1" strike="noStrike">
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1521,6 +1567,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1573,8 +1620,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="93412167"/>
-        <c:axId val="12559691"/>
+        <c:axId val="70986980"/>
+        <c:axId val="44374675"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1607,6 +1654,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1659,11 +1707,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="77116184"/>
-        <c:axId val="26030734"/>
+        <c:axId val="26318050"/>
+        <c:axId val="67620164"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93412167"/>
+        <c:axId val="70986980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1724,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1689,7 +1737,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1736,14 +1784,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12559691"/>
+        <c:crossAx val="44374675"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12559691"/>
+        <c:axId val="44374675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,7 +1813,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1778,7 +1826,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1796,7 +1844,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1825,11 +1873,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93412167"/>
+        <c:crossAx val="70986980"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="77116184"/>
+        <c:axId val="26318050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1842,7 +1890,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1855,7 +1903,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1902,14 +1950,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26030734"/>
+        <c:crossAx val="67620164"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26030734"/>
+        <c:axId val="67620164"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,7 +1970,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1935,7 +1983,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" spc="-1" strike="noStrike">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1953,7 +2001,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1982,7 +2030,1702 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77116184"/>
+        <c:crossAx val="26318050"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart94.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Floor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze!$G$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze!$G$11:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="9910826"/>
+        <c:axId val="22358397"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze!$H$10:$H$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Area</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze!$H$11:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="75873279"/>
+        <c:axId val="2830977"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="9910826"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22358397"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="22358397"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9910826"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="75873279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2830977"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2830977"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75873279"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart95.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Abs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze!$L$10:$L$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze!$L$11:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="28622036"/>
+        <c:axId val="88304639"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze!$M$10:$M$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Area</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze!$M$11:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="58846881"/>
+        <c:axId val="64332070"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="28622036"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88304639"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88304639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="28622036"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="58846881"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64332070"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="64332070"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="58846881"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart96.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Ceiling</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze!$L$10:$L$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze!$Q$11:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="13617406"/>
+        <c:axId val="50085370"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze!$M$10:$M$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Area</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze!$R$11:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="73404066"/>
+        <c:axId val="22713212"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="13617406"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50085370"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50085370"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="13617406"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="73404066"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22713212"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="22713212"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73404066"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -2012,16 +3755,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>797400</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2029,8 +3772,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2427120" y="2298240"/>
-        <a:ext cx="4059720" cy="2594520"/>
+        <a:off x="2474640" y="2289600"/>
+        <a:ext cx="4110120" cy="2594160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2042,16 +3785,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5760</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>805320</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9000</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2059,8 +3802,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6491160" y="2290680"/>
-        <a:ext cx="4067640" cy="2741400"/>
+        <a:off x="6589440" y="2282040"/>
+        <a:ext cx="4118040" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2073,15 +3816,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
+      <xdr:colOff>35280</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>797400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2089,8 +3832,103 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10574640" y="2299680"/>
-        <a:ext cx="4040280" cy="2741400"/>
+        <a:off x="10733760" y="2291040"/>
+        <a:ext cx="4080600" cy="2741040"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5760</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3297600" y="2614680"/>
+        <a:ext cx="4110120" cy="2594160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>5760</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7412400" y="2607120"/>
+        <a:ext cx="4118040" cy="2741040"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>35280</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>15480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="11556720" y="2616120"/>
+        <a:ext cx="4080600" cy="2741040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2108,15 +3946,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13:R13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,7 +3978,7 @@
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2327,6 +4165,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C10,0)</f>
         <v>8</v>
       </c>
       <c r="F10" s="10" t="n">
@@ -2399,6 +4238,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C11,0)</f>
         <v>10</v>
       </c>
       <c r="F11" s="10" t="n">
@@ -2490,6 +4330,41 @@
         <v>14.3333333333333</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="19" t="n">
+        <f aca="false">H13</f>
+        <v>8.33333333333333</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="19" t="n">
+        <f aca="false">M13</f>
+        <v>5.33333333333333</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="19" t="n">
+        <f aca="false">R13</f>
+        <v>14.3333333333333</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D7:H7"/>
@@ -2505,4 +4380,487 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S20"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6632653061225"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <f aca="false">B1/B5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <f aca="false">B3/2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <f aca="false">(B2-B1)/B3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <f aca="false">(B1+B2)/2*B3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f aca="false">B6/3</f>
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <f aca="false">$B$7*(A11+1)</f>
+        <v>33.3333333333333</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <f aca="false">-$F$1+SQRT($F$1*$F$1+2*B11/$B$5)</f>
+        <v>4.57427107756338</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <f aca="false">(B1+B1+B5*C11)*C11/2</f>
+        <v>33.3333333333333</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C11,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <f aca="false">F11-E11</f>
+        <v>4</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E11)+($B$1+$B$5*F11))/2*(F11-E11)</f>
+        <v>28</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <f aca="false">ABS(H11-$B$7)</f>
+        <v>5.33333333333334</v>
+      </c>
+      <c r="J11" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12" t="n">
+        <f aca="false">ROUND(C11,0)</f>
+        <v>5</v>
+      </c>
+      <c r="L11" s="12" t="n">
+        <f aca="false">K11-J11</f>
+        <v>5</v>
+      </c>
+      <c r="M11" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*J11)+($B$1+$B$5*K11))/2*(K11-J11)</f>
+        <v>37.5</v>
+      </c>
+      <c r="N11" s="13" t="n">
+        <f aca="false">ABS(M11-$B$7)</f>
+        <v>4.16666666666666</v>
+      </c>
+      <c r="O11" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="14" t="n">
+        <f aca="false">ROUNDUP(C11,0)</f>
+        <v>5</v>
+      </c>
+      <c r="Q11" s="14" t="n">
+        <f aca="false">P11-O11</f>
+        <v>5</v>
+      </c>
+      <c r="R11" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*O11)+($B$1+$B$5*P11))/2*(P11-O11)</f>
+        <v>37.5</v>
+      </c>
+      <c r="S11" s="9" t="n">
+        <f aca="false">ABS(R11-$B$7)</f>
+        <v>4.16666666666666</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <f aca="false">$B$7*(A12+1)</f>
+        <v>66.6666666666667</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <f aca="false">-$F$1+SQRT($F$1*$F$1+2*B12/$B$5)</f>
+        <v>7.58305739211792</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C12)*C12/2-SUM($D$11:D11)</f>
+        <v>33.3333333333333</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <f aca="false">F11</f>
+        <v>4</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C12,0)</f>
+        <v>7</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <f aca="false">F12-E12</f>
+        <v>3</v>
+      </c>
+      <c r="H12" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E12)+($B$1+$B$5*F12))/2*(F12-E12)</f>
+        <v>31.5</v>
+      </c>
+      <c r="I12" s="11" t="n">
+        <f aca="false">ABS(H12-$B$7)</f>
+        <v>1.83333333333334</v>
+      </c>
+      <c r="J12" s="12" t="n">
+        <f aca="false">K11</f>
+        <v>5</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">ROUND(C12,0)</f>
+        <v>8</v>
+      </c>
+      <c r="L12" s="12" t="n">
+        <f aca="false">K12-J12</f>
+        <v>3</v>
+      </c>
+      <c r="M12" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*J12)+($B$1+$B$5*K12))/2*(K12-J12)</f>
+        <v>34.5</v>
+      </c>
+      <c r="N12" s="13" t="n">
+        <f aca="false">ABS(M12-$B$7)</f>
+        <v>1.16666666666666</v>
+      </c>
+      <c r="O12" s="14" t="n">
+        <f aca="false">P11</f>
+        <v>5</v>
+      </c>
+      <c r="P12" s="14" t="n">
+        <f aca="false">ROUNDUP(C12,0)</f>
+        <v>8</v>
+      </c>
+      <c r="Q12" s="14" t="n">
+        <f aca="false">P12-O12</f>
+        <v>3</v>
+      </c>
+      <c r="R12" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*O12)+($B$1+$B$5*P12))/2*(P12-O12)</f>
+        <v>34.5</v>
+      </c>
+      <c r="S12" s="9" t="n">
+        <f aca="false">ABS(R12-$B$7)</f>
+        <v>1.16666666666666</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <f aca="false">$B$7*(A13+1)</f>
+        <v>100</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <f aca="false">-$F$1+SQRT($F$1*$F$1+2*B13/$B$5)</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C13)*C13/2-SUM($D$11:D12)</f>
+        <v>33.3333333333333</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <f aca="false">F12</f>
+        <v>7</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C13,0)</f>
+        <v>10</v>
+      </c>
+      <c r="G13" s="10" t="n">
+        <f aca="false">F13-E13</f>
+        <v>3</v>
+      </c>
+      <c r="H13" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E13)+($B$1+$B$5*F13))/2*(F13-E13)</f>
+        <v>40.5</v>
+      </c>
+      <c r="I13" s="11" t="n">
+        <f aca="false">ABS(H13-$B$7)</f>
+        <v>7.16666666666666</v>
+      </c>
+      <c r="J13" s="12" t="n">
+        <f aca="false">K12</f>
+        <v>8</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">ROUND(C13,0)</f>
+        <v>10</v>
+      </c>
+      <c r="L13" s="12" t="n">
+        <f aca="false">K13-J13</f>
+        <v>2</v>
+      </c>
+      <c r="M13" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*J13)+($B$1+$B$5*K13))/2*(K13-J13)</f>
+        <v>28</v>
+      </c>
+      <c r="N13" s="13" t="n">
+        <f aca="false">ABS(M13-$B$7)</f>
+        <v>5.33333333333334</v>
+      </c>
+      <c r="O13" s="14" t="n">
+        <f aca="false">P12</f>
+        <v>8</v>
+      </c>
+      <c r="P13" s="14" t="n">
+        <f aca="false">ROUNDUP(C13,0)</f>
+        <v>10</v>
+      </c>
+      <c r="Q13" s="14" t="n">
+        <f aca="false">P13-O13</f>
+        <v>2</v>
+      </c>
+      <c r="R13" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*O13)+($B$1+$B$5*P13))/2*(P13-O13)</f>
+        <v>28</v>
+      </c>
+      <c r="S13" s="9" t="n">
+        <f aca="false">ABS(R13-$B$7)</f>
+        <v>5.33333333333334</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="17" t="n">
+        <f aca="false">SUM(I11:I13)</f>
+        <v>14.3333333333333</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="17" t="n">
+        <f aca="false">SUM(N11:N13)</f>
+        <v>10.6666666666667</v>
+      </c>
+      <c r="R15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15" s="17" t="n">
+        <f aca="false">SUM(S11:S13)</f>
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="19" t="n">
+        <f aca="false">I15</f>
+        <v>14.3333333333333</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="19" t="n">
+        <f aca="false">N15</f>
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="19" t="n">
+        <f aca="false">S15</f>
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="O9:S9"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Results moved to individual folders
</commit_message>
<xml_diff>
--- a/source/gfoidl.Stochastics/Partitioners/Calcs.xlsx
+++ b/source/gfoidl.Stochastics/Partitioners/Calcs.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Triangle" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Trapeze" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Trapeze_16" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="21">
   <si>
     <t>N </t>
   </si>
@@ -81,6 +82,9 @@
   </si>
   <si>
     <t>Area exact</t>
+  </si>
+  <si>
+    <t>Delta</t>
   </si>
 </sst>
 </file>
@@ -361,7 +365,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart80.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -490,8 +494,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="71436269"/>
-        <c:axId val="70410611"/>
+        <c:axId val="13046782"/>
+        <c:axId val="2289086"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -577,11 +581,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="44846567"/>
-        <c:axId val="53326331"/>
+        <c:axId val="38835233"/>
+        <c:axId val="35856337"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71436269"/>
+        <c:axId val="13046782"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,14 +658,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70410611"/>
+        <c:crossAx val="2289086"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70410611"/>
+        <c:axId val="2289086"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,11 +747,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71436269"/>
+        <c:crossAx val="13046782"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="44846567"/>
+        <c:axId val="38835233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,14 +824,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53326331"/>
+        <c:crossAx val="35856337"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53326331"/>
+        <c:axId val="35856337"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +904,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44846567"/>
+        <c:crossAx val="38835233"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -926,7 +930,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart81.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1055,8 +1059,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="81619490"/>
-        <c:axId val="83193813"/>
+        <c:axId val="48624445"/>
+        <c:axId val="62794576"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1142,11 +1146,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="50071952"/>
-        <c:axId val="29861765"/>
+        <c:axId val="43660653"/>
+        <c:axId val="97943879"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81619490"/>
+        <c:axId val="48624445"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,14 +1223,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83193813"/>
+        <c:crossAx val="62794576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83193813"/>
+        <c:axId val="62794576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,11 +1312,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81619490"/>
+        <c:crossAx val="48624445"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="50071952"/>
+        <c:axId val="43660653"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,14 +1389,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29861765"/>
+        <c:crossAx val="97943879"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29861765"/>
+        <c:axId val="97943879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,7 +1469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50071952"/>
+        <c:crossAx val="43660653"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -1491,7 +1495,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart82.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1620,8 +1624,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="70986980"/>
-        <c:axId val="44374675"/>
+        <c:axId val="51371434"/>
+        <c:axId val="39335392"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1707,11 +1711,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="26318050"/>
-        <c:axId val="67620164"/>
+        <c:axId val="83474964"/>
+        <c:axId val="81905265"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70986980"/>
+        <c:axId val="51371434"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,14 +1788,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44374675"/>
+        <c:crossAx val="39335392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44374675"/>
+        <c:axId val="39335392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,11 +1877,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70986980"/>
+        <c:crossAx val="51371434"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="26318050"/>
+        <c:axId val="83474964"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,14 +1954,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67620164"/>
+        <c:crossAx val="81905265"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67620164"/>
+        <c:axId val="81905265"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,7 +2034,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26318050"/>
+        <c:crossAx val="83474964"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -2056,7 +2060,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart83.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2185,8 +2189,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="9910826"/>
-        <c:axId val="22358397"/>
+        <c:axId val="39830310"/>
+        <c:axId val="57298659"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2272,11 +2276,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="75873279"/>
-        <c:axId val="2830977"/>
+        <c:axId val="25944815"/>
+        <c:axId val="83873758"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="9910826"/>
+        <c:axId val="39830310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2349,14 +2353,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22358397"/>
+        <c:crossAx val="57298659"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22358397"/>
+        <c:axId val="57298659"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,11 +2442,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9910826"/>
+        <c:crossAx val="39830310"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="75873279"/>
+        <c:axId val="25944815"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2515,14 +2519,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2830977"/>
+        <c:crossAx val="83873758"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2830977"/>
+        <c:axId val="83873758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2595,7 +2599,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75873279"/>
+        <c:crossAx val="25944815"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -2621,7 +2625,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart84.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2750,8 +2754,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="28622036"/>
-        <c:axId val="88304639"/>
+        <c:axId val="66245737"/>
+        <c:axId val="78279124"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2837,11 +2841,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="58846881"/>
-        <c:axId val="64332070"/>
+        <c:axId val="71901507"/>
+        <c:axId val="71940078"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28622036"/>
+        <c:axId val="66245737"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2914,14 +2918,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88304639"/>
+        <c:crossAx val="78279124"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88304639"/>
+        <c:axId val="78279124"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3003,11 +3007,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28622036"/>
+        <c:crossAx val="66245737"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="58846881"/>
+        <c:axId val="71901507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3080,14 +3084,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64332070"/>
+        <c:crossAx val="71940078"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64332070"/>
+        <c:axId val="71940078"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3160,7 +3164,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58846881"/>
+        <c:crossAx val="71901507"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -3186,7 +3190,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart85.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3315,8 +3319,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="13617406"/>
-        <c:axId val="50085370"/>
+        <c:axId val="59242577"/>
+        <c:axId val="48707125"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3402,11 +3406,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="73404066"/>
-        <c:axId val="22713212"/>
+        <c:axId val="16643398"/>
+        <c:axId val="97185702"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13617406"/>
+        <c:axId val="59242577"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3479,14 +3483,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50085370"/>
+        <c:crossAx val="48707125"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50085370"/>
+        <c:axId val="48707125"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3568,11 +3572,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13617406"/>
+        <c:crossAx val="59242577"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="73404066"/>
+        <c:axId val="16643398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3645,14 +3649,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22713212"/>
+        <c:crossAx val="97185702"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22713212"/>
+        <c:axId val="97185702"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3725,7 +3729,2170 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73404066"/>
+        <c:crossAx val="16643398"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart86.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Floor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze_16!$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze_16!$A$11:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze_16!$G$11:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>5929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6078</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6597</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7028</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7277</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7556</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7869</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8225</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8633</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9674</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10360</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="21249848"/>
+        <c:axId val="36377086"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze_16!$I$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Delta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze_16!$A$11:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze_16!$I$11:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-170270.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>148746</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-163250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174570</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10204.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-39852</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30402</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-118274.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9727.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>73987.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-26525.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-74388</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18810</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="33831676"/>
+        <c:axId val="42581807"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="21249848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="36377086"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="36377086"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="21249848"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="33831676"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="42581807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="42581807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Delta abs Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="33831676"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart87.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Abs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze_16!$M$10:$M$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze_16!$A$11:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze_16!$M$11:$M$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>5930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6237</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6409</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6597</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7028</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7278</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7556</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7869</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8224</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8634</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9109</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9675</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10359</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="64748085"/>
+        <c:axId val="12706011"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze_16!$O$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Delta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze_16!$A$11:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze_16!$O$11:$O$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>73800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-95324.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68506.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-57186.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10204.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-39852</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30402</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79368</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7366</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-17596.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-108230</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>138834</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-75559.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72187.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-127765.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="8080425"/>
+        <c:axId val="61417441"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="64748085"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12706011"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="12706011"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64748085"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="8080425"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="61417441"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="61417441"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Delta abs Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8080425"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart88.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Ceiling</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze_16!$M$10:$M$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze_16!$A$11:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze_16!$S$11:$S$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>5930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6078</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6596</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7028</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7277</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7556</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7869</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8225</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8633</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9109</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9675</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10360</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="5160907"/>
+        <c:axId val="7109474"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trapeze_16!$U$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Delta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trapeze_16!$A$11:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trapeze_16!$U$11:$U$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>73800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>142668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-169486</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>168160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-215142</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>172095.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-125551.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7366</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-17596.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65762.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-35158.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-75559.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72187.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8450</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-80637.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="93330991"/>
+        <c:axId val="77410072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="5160907"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7109474"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="7109474"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="5160907"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="93330991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Partition Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="77410072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="77410072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Delta abs Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93330991"/>
         <c:crosses val="max"/>
       </c:valAx>
       <c:spPr>
@@ -3756,15 +5923,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:colOff>59760</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:colOff>54360</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3772,8 +5939,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2474640" y="2289600"/>
-        <a:ext cx="4110120" cy="2594160"/>
+        <a:off x="2574360" y="2271600"/>
+        <a:ext cx="4185360" cy="2593440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3786,15 +5953,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>59760</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>62280</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3802,8 +5969,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6589440" y="2282040"/>
-        <a:ext cx="4118040" cy="2741040"/>
+        <a:off x="6765120" y="2264040"/>
+        <a:ext cx="4193640" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3816,15 +5983,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>35280</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:colOff>89280</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3832,8 +5999,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10733760" y="2291040"/>
-        <a:ext cx="4080600" cy="2741040"/>
+        <a:off x="10985760" y="2273040"/>
+        <a:ext cx="4156200" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3851,15 +6018,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:colOff>59760</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:colOff>54360</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3867,8 +6034,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3297600" y="2614680"/>
-        <a:ext cx="4110120" cy="2594160"/>
+        <a:off x="3412440" y="2596680"/>
+        <a:ext cx="4185720" cy="2593440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3881,15 +6048,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>59760</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>62280</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3897,8 +6064,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7412400" y="2607120"/>
-        <a:ext cx="4118040" cy="2741040"/>
+        <a:off x="7603560" y="2589120"/>
+        <a:ext cx="4193280" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3911,15 +6078,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>35280</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:colOff>89280</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3927,8 +6094,103 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11556720" y="2616120"/>
-        <a:ext cx="4080600" cy="2741040"/>
+        <a:off x="11823840" y="2598120"/>
+        <a:ext cx="4156200" cy="2740320"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>60480</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>159120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>54720</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>150840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4205520" y="4710600"/>
+        <a:ext cx="5290200" cy="2592720"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>60120</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>63000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>127800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="9501120" y="4703040"/>
+        <a:ext cx="5321520" cy="2739960"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>90000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>160560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>54360</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>136800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="14849640" y="4712040"/>
+        <a:ext cx="5245200" cy="2739960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3954,7 +6216,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4389,13 +6651,13 @@
   </sheetPr>
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4856,7 +7118,1705 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:V33"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X34" activeCellId="0" sqref="X34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.984693877551"/>
+    <col collapsed="false" hidden="false" max="19" min="15" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.8775510204082"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>250000</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <f aca="false">B1/B5</f>
+        <v>-250000</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <f aca="false">B3/2</f>
+        <v>62500</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <f aca="false">(B2-B1)/B3</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <f aca="false">(B1+B2)/2*B3</f>
+        <v>23437500000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f aca="false">B6/16</f>
+        <v>1464843750</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="U10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <f aca="false">$B$7*(A11+1)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B11/$B$5)</f>
+        <v>5929.69762791705</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <f aca="false">(B1+B1+B5*C11)*C11/2</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C11,0)</f>
+        <v>5929</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <f aca="false">F11-E11</f>
+        <v>5929</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E11)+($B$1+$B$5*F11))/2*(F11-E11)</f>
+        <v>1464673479.5</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <f aca="false">H11-$B$7</f>
+        <v>-170270.5</v>
+      </c>
+      <c r="J11" s="11" t="n">
+        <f aca="false">ABS(H11-$B$7)</f>
+        <v>170270.5</v>
+      </c>
+      <c r="K11" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12" t="n">
+        <f aca="false">ROUND(C11,0)</f>
+        <v>5930</v>
+      </c>
+      <c r="M11" s="12" t="n">
+        <f aca="false">L11-K11</f>
+        <v>5930</v>
+      </c>
+      <c r="N11" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K11)+($B$1+$B$5*L11))/2*(L11-K11)</f>
+        <v>1464917550</v>
+      </c>
+      <c r="O11" s="13" t="n">
+        <f aca="false">N11-$B$7</f>
+        <v>73800</v>
+      </c>
+      <c r="P11" s="13" t="n">
+        <f aca="false">ABS(N11-$B$7)</f>
+        <v>73800</v>
+      </c>
+      <c r="Q11" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="14" t="n">
+        <f aca="false">ROUNDUP(C11,0)</f>
+        <v>5930</v>
+      </c>
+      <c r="S11" s="14" t="n">
+        <f aca="false">R11-Q11</f>
+        <v>5930</v>
+      </c>
+      <c r="T11" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q11)+($B$1+$B$5*R11))/2*(R11-Q11)</f>
+        <v>1464917550</v>
+      </c>
+      <c r="U11" s="15" t="n">
+        <f aca="false">T11-$B$7</f>
+        <v>73800</v>
+      </c>
+      <c r="V11" s="9" t="n">
+        <f aca="false">ABS(T11-$B$7)</f>
+        <v>73800</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <f aca="false">$B$7*(A12+1)</f>
+        <v>2929687500</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B12/$B$5)</f>
+        <v>12007.0904417529</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C12)*C12/2-SUM($D$11:D11)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <f aca="false">F11</f>
+        <v>5929</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C12,0)</f>
+        <v>12007</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <f aca="false">F12-E12</f>
+        <v>6078</v>
+      </c>
+      <c r="H12" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E12)+($B$1+$B$5*F12))/2*(F12-E12)</f>
+        <v>1464992496</v>
+      </c>
+      <c r="I12" s="11" t="n">
+        <f aca="false">H12-$B$7</f>
+        <v>148746</v>
+      </c>
+      <c r="J12" s="11" t="n">
+        <f aca="false">ABS(H12-$B$7)</f>
+        <v>148746</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">L11</f>
+        <v>5930</v>
+      </c>
+      <c r="L12" s="12" t="n">
+        <f aca="false">ROUND(C12,0)</f>
+        <v>12007</v>
+      </c>
+      <c r="M12" s="12" t="n">
+        <f aca="false">L12-K12</f>
+        <v>6077</v>
+      </c>
+      <c r="N12" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K12)+($B$1+$B$5*L12))/2*(L12-K12)</f>
+        <v>1464748425.5</v>
+      </c>
+      <c r="O12" s="13" t="n">
+        <f aca="false">N12-$B$7</f>
+        <v>-95324.5</v>
+      </c>
+      <c r="P12" s="13" t="n">
+        <f aca="false">ABS(N12-$B$7)</f>
+        <v>95324.5</v>
+      </c>
+      <c r="Q12" s="14" t="n">
+        <f aca="false">R11</f>
+        <v>5930</v>
+      </c>
+      <c r="R12" s="14" t="n">
+        <f aca="false">ROUNDUP(C12,0)</f>
+        <v>12008</v>
+      </c>
+      <c r="S12" s="14" t="n">
+        <f aca="false">R12-Q12</f>
+        <v>6078</v>
+      </c>
+      <c r="T12" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q12)+($B$1+$B$5*R12))/2*(R12-Q12)</f>
+        <v>1464986418</v>
+      </c>
+      <c r="U12" s="15" t="n">
+        <f aca="false">T12-$B$7</f>
+        <v>142668</v>
+      </c>
+      <c r="V12" s="9" t="n">
+        <f aca="false">ABS(T12-$B$7)</f>
+        <v>142668</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <f aca="false">$B$7*(A13+1)</f>
+        <v>4394531250</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B13/$B$5)</f>
+        <v>18243.7972782605</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C13)*C13/2-SUM($D$11:D12)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <f aca="false">F12</f>
+        <v>12007</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C13,0)</f>
+        <v>18243</v>
+      </c>
+      <c r="G13" s="10" t="n">
+        <f aca="false">F13-E13</f>
+        <v>6236</v>
+      </c>
+      <c r="H13" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E13)+($B$1+$B$5*F13))/2*(F13-E13)</f>
+        <v>1464680500</v>
+      </c>
+      <c r="I13" s="11" t="n">
+        <f aca="false">H13-$B$7</f>
+        <v>-163250</v>
+      </c>
+      <c r="J13" s="11" t="n">
+        <f aca="false">ABS(H13-$B$7)</f>
+        <v>163250</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">L12</f>
+        <v>12007</v>
+      </c>
+      <c r="L13" s="12" t="n">
+        <f aca="false">ROUND(C13,0)</f>
+        <v>18244</v>
+      </c>
+      <c r="M13" s="12" t="n">
+        <f aca="false">L13-K13</f>
+        <v>6237</v>
+      </c>
+      <c r="N13" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K13)+($B$1+$B$5*L13))/2*(L13-K13)</f>
+        <v>1464912256.5</v>
+      </c>
+      <c r="O13" s="13" t="n">
+        <f aca="false">N13-$B$7</f>
+        <v>68506.5</v>
+      </c>
+      <c r="P13" s="13" t="n">
+        <f aca="false">ABS(N13-$B$7)</f>
+        <v>68506.5</v>
+      </c>
+      <c r="Q13" s="14" t="n">
+        <f aca="false">R12</f>
+        <v>12008</v>
+      </c>
+      <c r="R13" s="14" t="n">
+        <f aca="false">ROUNDUP(C13,0)</f>
+        <v>18244</v>
+      </c>
+      <c r="S13" s="14" t="n">
+        <f aca="false">R13-Q13</f>
+        <v>6236</v>
+      </c>
+      <c r="T13" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q13)+($B$1+$B$5*R13))/2*(R13-Q13)</f>
+        <v>1464674264</v>
+      </c>
+      <c r="U13" s="15" t="n">
+        <f aca="false">T13-$B$7</f>
+        <v>-169486</v>
+      </c>
+      <c r="V13" s="9" t="n">
+        <f aca="false">ABS(T13-$B$7)</f>
+        <v>169486</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <f aca="false">$B$7*(A14+1)</f>
+        <v>5859375000</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B14/$B$5)</f>
+        <v>24653.0452835007</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C14)*C14/2-SUM($D$11:D13)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <f aca="false">F13</f>
+        <v>18243</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C14,0)</f>
+        <v>24653</v>
+      </c>
+      <c r="G14" s="10" t="n">
+        <f aca="false">F14-E14</f>
+        <v>6410</v>
+      </c>
+      <c r="H14" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E14)+($B$1+$B$5*F14))/2*(F14-E14)</f>
+        <v>1465018320</v>
+      </c>
+      <c r="I14" s="11" t="n">
+        <f aca="false">H14-$B$7</f>
+        <v>174570</v>
+      </c>
+      <c r="J14" s="11" t="n">
+        <f aca="false">ABS(H14-$B$7)</f>
+        <v>174570</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">L13</f>
+        <v>18244</v>
+      </c>
+      <c r="L14" s="12" t="n">
+        <f aca="false">ROUND(C14,0)</f>
+        <v>24653</v>
+      </c>
+      <c r="M14" s="12" t="n">
+        <f aca="false">L14-K14</f>
+        <v>6409</v>
+      </c>
+      <c r="N14" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K14)+($B$1+$B$5*L14))/2*(L14-K14)</f>
+        <v>1464786563.5</v>
+      </c>
+      <c r="O14" s="13" t="n">
+        <f aca="false">N14-$B$7</f>
+        <v>-57186.5</v>
+      </c>
+      <c r="P14" s="13" t="n">
+        <f aca="false">ABS(N14-$B$7)</f>
+        <v>57186.5</v>
+      </c>
+      <c r="Q14" s="14" t="n">
+        <f aca="false">R13</f>
+        <v>18244</v>
+      </c>
+      <c r="R14" s="14" t="n">
+        <f aca="false">ROUNDUP(C14,0)</f>
+        <v>24654</v>
+      </c>
+      <c r="S14" s="14" t="n">
+        <f aca="false">R14-Q14</f>
+        <v>6410</v>
+      </c>
+      <c r="T14" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q14)+($B$1+$B$5*R14))/2*(R14-Q14)</f>
+        <v>1465011910</v>
+      </c>
+      <c r="U14" s="15" t="n">
+        <f aca="false">T14-$B$7</f>
+        <v>168160</v>
+      </c>
+      <c r="V14" s="9" t="n">
+        <f aca="false">ABS(T14-$B$7)</f>
+        <v>168160</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <f aca="false">$B$7*(A15+1)</f>
+        <v>7324218750</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B15/$B$5)</f>
+        <v>31250</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C15)*C15/2-SUM($D$11:D14)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <f aca="false">F14</f>
+        <v>24653</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C15,0)</f>
+        <v>31250</v>
+      </c>
+      <c r="G15" s="10" t="n">
+        <f aca="false">F15-E15</f>
+        <v>6597</v>
+      </c>
+      <c r="H15" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E15)+($B$1+$B$5*F15))/2*(F15-E15)</f>
+        <v>1464853954.5</v>
+      </c>
+      <c r="I15" s="11" t="n">
+        <f aca="false">H15-$B$7</f>
+        <v>10204.5</v>
+      </c>
+      <c r="J15" s="11" t="n">
+        <f aca="false">ABS(H15-$B$7)</f>
+        <v>10204.5</v>
+      </c>
+      <c r="K15" s="12" t="n">
+        <f aca="false">L14</f>
+        <v>24653</v>
+      </c>
+      <c r="L15" s="12" t="n">
+        <f aca="false">ROUND(C15,0)</f>
+        <v>31250</v>
+      </c>
+      <c r="M15" s="12" t="n">
+        <f aca="false">L15-K15</f>
+        <v>6597</v>
+      </c>
+      <c r="N15" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K15)+($B$1+$B$5*L15))/2*(L15-K15)</f>
+        <v>1464853954.5</v>
+      </c>
+      <c r="O15" s="13" t="n">
+        <f aca="false">N15-$B$7</f>
+        <v>10204.5</v>
+      </c>
+      <c r="P15" s="13" t="n">
+        <f aca="false">ABS(N15-$B$7)</f>
+        <v>10204.5</v>
+      </c>
+      <c r="Q15" s="14" t="n">
+        <f aca="false">R14</f>
+        <v>24654</v>
+      </c>
+      <c r="R15" s="14" t="n">
+        <f aca="false">ROUNDUP(C15,0)</f>
+        <v>31250</v>
+      </c>
+      <c r="S15" s="14" t="n">
+        <f aca="false">R15-Q15</f>
+        <v>6596</v>
+      </c>
+      <c r="T15" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q15)+($B$1+$B$5*R15))/2*(R15-Q15)</f>
+        <v>1464628608</v>
+      </c>
+      <c r="U15" s="15" t="n">
+        <f aca="false">T15-$B$7</f>
+        <v>-215142</v>
+      </c>
+      <c r="V15" s="9" t="n">
+        <f aca="false">ABS(T15-$B$7)</f>
+        <v>215142</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <f aca="false">$B$7*(A16+1)</f>
+        <v>8789062500</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B16/$B$5)</f>
+        <v>38052.1880273354</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C16)*C16/2-SUM($D$11:D15)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <f aca="false">F15</f>
+        <v>31250</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C16,0)</f>
+        <v>38052</v>
+      </c>
+      <c r="G16" s="10" t="n">
+        <f aca="false">F16-E16</f>
+        <v>6802</v>
+      </c>
+      <c r="H16" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E16)+($B$1+$B$5*F16))/2*(F16-E16)</f>
+        <v>1464803898</v>
+      </c>
+      <c r="I16" s="11" t="n">
+        <f aca="false">H16-$B$7</f>
+        <v>-39852</v>
+      </c>
+      <c r="J16" s="11" t="n">
+        <f aca="false">ABS(H16-$B$7)</f>
+        <v>39852</v>
+      </c>
+      <c r="K16" s="12" t="n">
+        <f aca="false">L15</f>
+        <v>31250</v>
+      </c>
+      <c r="L16" s="12" t="n">
+        <f aca="false">ROUND(C16,0)</f>
+        <v>38052</v>
+      </c>
+      <c r="M16" s="12" t="n">
+        <f aca="false">L16-K16</f>
+        <v>6802</v>
+      </c>
+      <c r="N16" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K16)+($B$1+$B$5*L16))/2*(L16-K16)</f>
+        <v>1464803898</v>
+      </c>
+      <c r="O16" s="13" t="n">
+        <f aca="false">N16-$B$7</f>
+        <v>-39852</v>
+      </c>
+      <c r="P16" s="13" t="n">
+        <f aca="false">ABS(N16-$B$7)</f>
+        <v>39852</v>
+      </c>
+      <c r="Q16" s="14" t="n">
+        <f aca="false">R15</f>
+        <v>31250</v>
+      </c>
+      <c r="R16" s="14" t="n">
+        <f aca="false">ROUNDUP(C16,0)</f>
+        <v>38053</v>
+      </c>
+      <c r="S16" s="14" t="n">
+        <f aca="false">R16-Q16</f>
+        <v>6803</v>
+      </c>
+      <c r="T16" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q16)+($B$1+$B$5*R16))/2*(R16-Q16)</f>
+        <v>1465015845.5</v>
+      </c>
+      <c r="U16" s="15" t="n">
+        <f aca="false">T16-$B$7</f>
+        <v>172095.5</v>
+      </c>
+      <c r="V16" s="9" t="n">
+        <f aca="false">ABS(T16-$B$7)</f>
+        <v>172095.5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <f aca="false">$B$7*(A17+1)</f>
+        <v>10253906250</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B17/$B$5)</f>
+        <v>45080.0461155625</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C17)*C17/2-SUM($D$11:D16)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <f aca="false">F16</f>
+        <v>38052</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C17,0)</f>
+        <v>45080</v>
+      </c>
+      <c r="G17" s="10" t="n">
+        <f aca="false">F17-E17</f>
+        <v>7028</v>
+      </c>
+      <c r="H17" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E17)+($B$1+$B$5*F17))/2*(F17-E17)</f>
+        <v>1464874152</v>
+      </c>
+      <c r="I17" s="11" t="n">
+        <f aca="false">H17-$B$7</f>
+        <v>30402</v>
+      </c>
+      <c r="J17" s="11" t="n">
+        <f aca="false">ABS(H17-$B$7)</f>
+        <v>30402</v>
+      </c>
+      <c r="K17" s="12" t="n">
+        <f aca="false">L16</f>
+        <v>38052</v>
+      </c>
+      <c r="L17" s="12" t="n">
+        <f aca="false">ROUND(C17,0)</f>
+        <v>45080</v>
+      </c>
+      <c r="M17" s="12" t="n">
+        <f aca="false">L17-K17</f>
+        <v>7028</v>
+      </c>
+      <c r="N17" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K17)+($B$1+$B$5*L17))/2*(L17-K17)</f>
+        <v>1464874152</v>
+      </c>
+      <c r="O17" s="13" t="n">
+        <f aca="false">N17-$B$7</f>
+        <v>30402</v>
+      </c>
+      <c r="P17" s="13" t="n">
+        <f aca="false">ABS(N17-$B$7)</f>
+        <v>30402</v>
+      </c>
+      <c r="Q17" s="14" t="n">
+        <f aca="false">R16</f>
+        <v>38053</v>
+      </c>
+      <c r="R17" s="14" t="n">
+        <f aca="false">ROUNDUP(C17,0)</f>
+        <v>45081</v>
+      </c>
+      <c r="S17" s="14" t="n">
+        <f aca="false">R17-Q17</f>
+        <v>7028</v>
+      </c>
+      <c r="T17" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q17)+($B$1+$B$5*R17))/2*(R17-Q17)</f>
+        <v>1464867124</v>
+      </c>
+      <c r="U17" s="15" t="n">
+        <f aca="false">T17-$B$7</f>
+        <v>23374</v>
+      </c>
+      <c r="V17" s="9" t="n">
+        <f aca="false">ABS(T17-$B$7)</f>
+        <v>23374</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <f aca="false">$B$7*(A18+1)</f>
+        <v>11718750000</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B18/$B$5)</f>
+        <v>52357.6462394763</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C18)*C18/2-SUM($D$11:D17)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <f aca="false">F17</f>
+        <v>45080</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C18,0)</f>
+        <v>52357</v>
+      </c>
+      <c r="G18" s="10" t="n">
+        <f aca="false">F18-E18</f>
+        <v>7277</v>
+      </c>
+      <c r="H18" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E18)+($B$1+$B$5*F18))/2*(F18-E18)</f>
+        <v>1464725475.5</v>
+      </c>
+      <c r="I18" s="11" t="n">
+        <f aca="false">H18-$B$7</f>
+        <v>-118274.5</v>
+      </c>
+      <c r="J18" s="11" t="n">
+        <f aca="false">ABS(H18-$B$7)</f>
+        <v>118274.5</v>
+      </c>
+      <c r="K18" s="12" t="n">
+        <f aca="false">L17</f>
+        <v>45080</v>
+      </c>
+      <c r="L18" s="12" t="n">
+        <f aca="false">ROUND(C18,0)</f>
+        <v>52358</v>
+      </c>
+      <c r="M18" s="12" t="n">
+        <f aca="false">L18-K18</f>
+        <v>7278</v>
+      </c>
+      <c r="N18" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K18)+($B$1+$B$5*L18))/2*(L18-K18)</f>
+        <v>1464923118</v>
+      </c>
+      <c r="O18" s="13" t="n">
+        <f aca="false">N18-$B$7</f>
+        <v>79368</v>
+      </c>
+      <c r="P18" s="13" t="n">
+        <f aca="false">ABS(N18-$B$7)</f>
+        <v>79368</v>
+      </c>
+      <c r="Q18" s="14" t="n">
+        <f aca="false">R17</f>
+        <v>45081</v>
+      </c>
+      <c r="R18" s="14" t="n">
+        <f aca="false">ROUNDUP(C18,0)</f>
+        <v>52358</v>
+      </c>
+      <c r="S18" s="14" t="n">
+        <f aca="false">R18-Q18</f>
+        <v>7277</v>
+      </c>
+      <c r="T18" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q18)+($B$1+$B$5*R18))/2*(R18-Q18)</f>
+        <v>1464718198.5</v>
+      </c>
+      <c r="U18" s="15" t="n">
+        <f aca="false">T18-$B$7</f>
+        <v>-125551.5</v>
+      </c>
+      <c r="V18" s="9" t="n">
+        <f aca="false">ABS(T18-$B$7)</f>
+        <v>125551.5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <f aca="false">$B$7*(A19+1)</f>
+        <v>13183593750</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B19/$B$5)</f>
+        <v>59913.6709281806</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C19)*C19/2-SUM($D$11:D18)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <f aca="false">F18</f>
+        <v>52357</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C19,0)</f>
+        <v>59913</v>
+      </c>
+      <c r="G19" s="10" t="n">
+        <f aca="false">F19-E19</f>
+        <v>7556</v>
+      </c>
+      <c r="H19" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E19)+($B$1+$B$5*F19))/2*(F19-E19)</f>
+        <v>1464843940</v>
+      </c>
+      <c r="I19" s="11" t="n">
+        <f aca="false">H19-$B$7</f>
+        <v>190</v>
+      </c>
+      <c r="J19" s="11" t="n">
+        <f aca="false">ABS(H19-$B$7)</f>
+        <v>190</v>
+      </c>
+      <c r="K19" s="12" t="n">
+        <f aca="false">L18</f>
+        <v>52358</v>
+      </c>
+      <c r="L19" s="12" t="n">
+        <f aca="false">ROUND(C19,0)</f>
+        <v>59914</v>
+      </c>
+      <c r="M19" s="12" t="n">
+        <f aca="false">L19-K19</f>
+        <v>7556</v>
+      </c>
+      <c r="N19" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K19)+($B$1+$B$5*L19))/2*(L19-K19)</f>
+        <v>1464836384</v>
+      </c>
+      <c r="O19" s="13" t="n">
+        <f aca="false">N19-$B$7</f>
+        <v>-7366</v>
+      </c>
+      <c r="P19" s="13" t="n">
+        <f aca="false">ABS(N19-$B$7)</f>
+        <v>7366</v>
+      </c>
+      <c r="Q19" s="14" t="n">
+        <f aca="false">R18</f>
+        <v>52358</v>
+      </c>
+      <c r="R19" s="14" t="n">
+        <f aca="false">ROUNDUP(C19,0)</f>
+        <v>59914</v>
+      </c>
+      <c r="S19" s="14" t="n">
+        <f aca="false">R19-Q19</f>
+        <v>7556</v>
+      </c>
+      <c r="T19" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q19)+($B$1+$B$5*R19))/2*(R19-Q19)</f>
+        <v>1464836384</v>
+      </c>
+      <c r="U19" s="15" t="n">
+        <f aca="false">T19-$B$7</f>
+        <v>-7366</v>
+      </c>
+      <c r="V19" s="9" t="n">
+        <f aca="false">ABS(T19-$B$7)</f>
+        <v>7366</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <f aca="false">$B$7*(A20+1)</f>
+        <v>14648437500</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B20/$B$5)</f>
+        <v>67782.7532860844</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C20)*C20/2-SUM($D$11:D19)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <f aca="false">F19</f>
+        <v>59913</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C20,0)</f>
+        <v>67782</v>
+      </c>
+      <c r="G20" s="10" t="n">
+        <f aca="false">F20-E20</f>
+        <v>7869</v>
+      </c>
+      <c r="H20" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E20)+($B$1+$B$5*F20))/2*(F20-E20)</f>
+        <v>1464834022.5</v>
+      </c>
+      <c r="I20" s="11" t="n">
+        <f aca="false">H20-$B$7</f>
+        <v>-9727.5</v>
+      </c>
+      <c r="J20" s="11" t="n">
+        <f aca="false">ABS(H20-$B$7)</f>
+        <v>9727.5</v>
+      </c>
+      <c r="K20" s="12" t="n">
+        <f aca="false">L19</f>
+        <v>59914</v>
+      </c>
+      <c r="L20" s="12" t="n">
+        <f aca="false">ROUND(C20,0)</f>
+        <v>67783</v>
+      </c>
+      <c r="M20" s="12" t="n">
+        <f aca="false">L20-K20</f>
+        <v>7869</v>
+      </c>
+      <c r="N20" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K20)+($B$1+$B$5*L20))/2*(L20-K20)</f>
+        <v>1464826153.5</v>
+      </c>
+      <c r="O20" s="13" t="n">
+        <f aca="false">N20-$B$7</f>
+        <v>-17596.5</v>
+      </c>
+      <c r="P20" s="13" t="n">
+        <f aca="false">ABS(N20-$B$7)</f>
+        <v>17596.5</v>
+      </c>
+      <c r="Q20" s="14" t="n">
+        <f aca="false">R19</f>
+        <v>59914</v>
+      </c>
+      <c r="R20" s="14" t="n">
+        <f aca="false">ROUNDUP(C20,0)</f>
+        <v>67783</v>
+      </c>
+      <c r="S20" s="14" t="n">
+        <f aca="false">R20-Q20</f>
+        <v>7869</v>
+      </c>
+      <c r="T20" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q20)+($B$1+$B$5*R20))/2*(R20-Q20)</f>
+        <v>1464826153.5</v>
+      </c>
+      <c r="U20" s="15" t="n">
+        <f aca="false">T20-$B$7</f>
+        <v>-17596.5</v>
+      </c>
+      <c r="V20" s="9" t="n">
+        <f aca="false">ABS(T20-$B$7)</f>
+        <v>17596.5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <f aca="false">$B$7*(A21+1)</f>
+        <v>16113281250</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B21/$B$5)</f>
+        <v>76007.3636615618</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C21)*C21/2-SUM($D$11:D20)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <f aca="false">F20</f>
+        <v>67782</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C21,0)</f>
+        <v>76007</v>
+      </c>
+      <c r="G21" s="10" t="n">
+        <f aca="false">F21-E21</f>
+        <v>8225</v>
+      </c>
+      <c r="H21" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E21)+($B$1+$B$5*F21))/2*(F21-E21)</f>
+        <v>1464917737.5</v>
+      </c>
+      <c r="I21" s="11" t="n">
+        <f aca="false">H21-$B$7</f>
+        <v>73987.5</v>
+      </c>
+      <c r="J21" s="11" t="n">
+        <f aca="false">ABS(H21-$B$7)</f>
+        <v>73987.5</v>
+      </c>
+      <c r="K21" s="12" t="n">
+        <f aca="false">L20</f>
+        <v>67783</v>
+      </c>
+      <c r="L21" s="12" t="n">
+        <f aca="false">ROUND(C21,0)</f>
+        <v>76007</v>
+      </c>
+      <c r="M21" s="12" t="n">
+        <f aca="false">L21-K21</f>
+        <v>8224</v>
+      </c>
+      <c r="N21" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K21)+($B$1+$B$5*L21))/2*(L21-K21)</f>
+        <v>1464735520</v>
+      </c>
+      <c r="O21" s="13" t="n">
+        <f aca="false">N21-$B$7</f>
+        <v>-108230</v>
+      </c>
+      <c r="P21" s="13" t="n">
+        <f aca="false">ABS(N21-$B$7)</f>
+        <v>108230</v>
+      </c>
+      <c r="Q21" s="14" t="n">
+        <f aca="false">R20</f>
+        <v>67783</v>
+      </c>
+      <c r="R21" s="14" t="n">
+        <f aca="false">ROUNDUP(C21,0)</f>
+        <v>76008</v>
+      </c>
+      <c r="S21" s="14" t="n">
+        <f aca="false">R21-Q21</f>
+        <v>8225</v>
+      </c>
+      <c r="T21" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q21)+($B$1+$B$5*R21))/2*(R21-Q21)</f>
+        <v>1464909512.5</v>
+      </c>
+      <c r="U21" s="15" t="n">
+        <f aca="false">T21-$B$7</f>
+        <v>65762.5</v>
+      </c>
+      <c r="V21" s="9" t="n">
+        <f aca="false">ABS(T21-$B$7)</f>
+        <v>65762.5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <f aca="false">$B$7*(A22+1)</f>
+        <v>17578125000</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B22/$B$5)</f>
+        <v>84640.5430584631</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C22)*C22/2-SUM($D$11:D21)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E22" s="7" t="n">
+        <f aca="false">F21</f>
+        <v>76007</v>
+      </c>
+      <c r="F22" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C22,0)</f>
+        <v>84640</v>
+      </c>
+      <c r="G22" s="10" t="n">
+        <f aca="false">F22-E22</f>
+        <v>8633</v>
+      </c>
+      <c r="H22" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E22)+($B$1+$B$5*F22))/2*(F22-E22)</f>
+        <v>1464817224.5</v>
+      </c>
+      <c r="I22" s="11" t="n">
+        <f aca="false">H22-$B$7</f>
+        <v>-26525.5</v>
+      </c>
+      <c r="J22" s="11" t="n">
+        <f aca="false">ABS(H22-$B$7)</f>
+        <v>26525.5</v>
+      </c>
+      <c r="K22" s="12" t="n">
+        <f aca="false">L21</f>
+        <v>76007</v>
+      </c>
+      <c r="L22" s="12" t="n">
+        <f aca="false">ROUND(C22,0)</f>
+        <v>84641</v>
+      </c>
+      <c r="M22" s="12" t="n">
+        <f aca="false">L22-K22</f>
+        <v>8634</v>
+      </c>
+      <c r="N22" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K22)+($B$1+$B$5*L22))/2*(L22-K22)</f>
+        <v>1464982584</v>
+      </c>
+      <c r="O22" s="13" t="n">
+        <f aca="false">N22-$B$7</f>
+        <v>138834</v>
+      </c>
+      <c r="P22" s="13" t="n">
+        <f aca="false">ABS(N22-$B$7)</f>
+        <v>138834</v>
+      </c>
+      <c r="Q22" s="14" t="n">
+        <f aca="false">R21</f>
+        <v>76008</v>
+      </c>
+      <c r="R22" s="14" t="n">
+        <f aca="false">ROUNDUP(C22,0)</f>
+        <v>84641</v>
+      </c>
+      <c r="S22" s="14" t="n">
+        <f aca="false">R22-Q22</f>
+        <v>8633</v>
+      </c>
+      <c r="T22" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q22)+($B$1+$B$5*R22))/2*(R22-Q22)</f>
+        <v>1464808591.5</v>
+      </c>
+      <c r="U22" s="15" t="n">
+        <f aca="false">T22-$B$7</f>
+        <v>-35158.5</v>
+      </c>
+      <c r="V22" s="9" t="n">
+        <f aca="false">ABS(T22-$B$7)</f>
+        <v>35158.5</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <f aca="false">$B$7*(A23+1)</f>
+        <v>19042968750</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B23/$B$5)</f>
+        <v>93750</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C23)*C23/2-SUM($D$11:D22)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <f aca="false">F22</f>
+        <v>84640</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C23,0)</f>
+        <v>93750</v>
+      </c>
+      <c r="G23" s="10" t="n">
+        <f aca="false">F23-E23</f>
+        <v>9110</v>
+      </c>
+      <c r="H23" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E23)+($B$1+$B$5*F23))/2*(F23-E23)</f>
+        <v>1464933550</v>
+      </c>
+      <c r="I23" s="11" t="n">
+        <f aca="false">H23-$B$7</f>
+        <v>89800</v>
+      </c>
+      <c r="J23" s="11" t="n">
+        <f aca="false">ABS(H23-$B$7)</f>
+        <v>89800</v>
+      </c>
+      <c r="K23" s="12" t="n">
+        <f aca="false">L22</f>
+        <v>84641</v>
+      </c>
+      <c r="L23" s="12" t="n">
+        <f aca="false">ROUND(C23,0)</f>
+        <v>93750</v>
+      </c>
+      <c r="M23" s="12" t="n">
+        <f aca="false">L23-K23</f>
+        <v>9109</v>
+      </c>
+      <c r="N23" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K23)+($B$1+$B$5*L23))/2*(L23-K23)</f>
+        <v>1464768190.5</v>
+      </c>
+      <c r="O23" s="13" t="n">
+        <f aca="false">N23-$B$7</f>
+        <v>-75559.5</v>
+      </c>
+      <c r="P23" s="13" t="n">
+        <f aca="false">ABS(N23-$B$7)</f>
+        <v>75559.5</v>
+      </c>
+      <c r="Q23" s="14" t="n">
+        <f aca="false">R22</f>
+        <v>84641</v>
+      </c>
+      <c r="R23" s="14" t="n">
+        <f aca="false">ROUNDUP(C23,0)</f>
+        <v>93750</v>
+      </c>
+      <c r="S23" s="14" t="n">
+        <f aca="false">R23-Q23</f>
+        <v>9109</v>
+      </c>
+      <c r="T23" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q23)+($B$1+$B$5*R23))/2*(R23-Q23)</f>
+        <v>1464768190.5</v>
+      </c>
+      <c r="U23" s="15" t="n">
+        <f aca="false">T23-$B$7</f>
+        <v>-75559.5</v>
+      </c>
+      <c r="V23" s="9" t="n">
+        <f aca="false">ABS(T23-$B$7)</f>
+        <v>75559.5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <f aca="false">$B$7*(A24+1)</f>
+        <v>20507812500</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B24/$B$5)</f>
+        <v>103424.507505518</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C24)*C24/2-SUM($D$11:D23)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <f aca="false">F23</f>
+        <v>93750</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C24,0)</f>
+        <v>103424</v>
+      </c>
+      <c r="G24" s="10" t="n">
+        <f aca="false">F24-E24</f>
+        <v>9674</v>
+      </c>
+      <c r="H24" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E24)+($B$1+$B$5*F24))/2*(F24-E24)</f>
+        <v>1464769362</v>
+      </c>
+      <c r="I24" s="11" t="n">
+        <f aca="false">H24-$B$7</f>
+        <v>-74388</v>
+      </c>
+      <c r="J24" s="11" t="n">
+        <f aca="false">ABS(H24-$B$7)</f>
+        <v>74388</v>
+      </c>
+      <c r="K24" s="12" t="n">
+        <f aca="false">L23</f>
+        <v>93750</v>
+      </c>
+      <c r="L24" s="12" t="n">
+        <f aca="false">ROUND(C24,0)</f>
+        <v>103425</v>
+      </c>
+      <c r="M24" s="12" t="n">
+        <f aca="false">L24-K24</f>
+        <v>9675</v>
+      </c>
+      <c r="N24" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K24)+($B$1+$B$5*L24))/2*(L24-K24)</f>
+        <v>1464915937.5</v>
+      </c>
+      <c r="O24" s="13" t="n">
+        <f aca="false">N24-$B$7</f>
+        <v>72187.5</v>
+      </c>
+      <c r="P24" s="13" t="n">
+        <f aca="false">ABS(N24-$B$7)</f>
+        <v>72187.5</v>
+      </c>
+      <c r="Q24" s="14" t="n">
+        <f aca="false">R23</f>
+        <v>93750</v>
+      </c>
+      <c r="R24" s="14" t="n">
+        <f aca="false">ROUNDUP(C24,0)</f>
+        <v>103425</v>
+      </c>
+      <c r="S24" s="14" t="n">
+        <f aca="false">R24-Q24</f>
+        <v>9675</v>
+      </c>
+      <c r="T24" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q24)+($B$1+$B$5*R24))/2*(R24-Q24)</f>
+        <v>1464915937.5</v>
+      </c>
+      <c r="U24" s="15" t="n">
+        <f aca="false">T24-$B$7</f>
+        <v>72187.5</v>
+      </c>
+      <c r="V24" s="9" t="n">
+        <f aca="false">ABS(T24-$B$7)</f>
+        <v>72187.5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <f aca="false">$B$7*(A25+1)</f>
+        <v>21972656250</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B25/$B$5)</f>
+        <v>113784.408014354</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C25)*C25/2-SUM($D$11:D24)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <f aca="false">F24</f>
+        <v>103424</v>
+      </c>
+      <c r="F25" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C25,0)</f>
+        <v>113784</v>
+      </c>
+      <c r="G25" s="10" t="n">
+        <f aca="false">F25-E25</f>
+        <v>10360</v>
+      </c>
+      <c r="H25" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E25)+($B$1+$B$5*F25))/2*(F25-E25)</f>
+        <v>1464862560</v>
+      </c>
+      <c r="I25" s="11" t="n">
+        <f aca="false">H25-$B$7</f>
+        <v>18810</v>
+      </c>
+      <c r="J25" s="11" t="n">
+        <f aca="false">ABS(H25-$B$7)</f>
+        <v>18810</v>
+      </c>
+      <c r="K25" s="12" t="n">
+        <f aca="false">L24</f>
+        <v>103425</v>
+      </c>
+      <c r="L25" s="12" t="n">
+        <f aca="false">ROUND(C25,0)</f>
+        <v>113784</v>
+      </c>
+      <c r="M25" s="12" t="n">
+        <f aca="false">L25-K25</f>
+        <v>10359</v>
+      </c>
+      <c r="N25" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K25)+($B$1+$B$5*L25))/2*(L25-K25)</f>
+        <v>1464715984.5</v>
+      </c>
+      <c r="O25" s="13" t="n">
+        <f aca="false">N25-$B$7</f>
+        <v>-127765.5</v>
+      </c>
+      <c r="P25" s="13" t="n">
+        <f aca="false">ABS(N25-$B$7)</f>
+        <v>127765.5</v>
+      </c>
+      <c r="Q25" s="14" t="n">
+        <f aca="false">R24</f>
+        <v>103425</v>
+      </c>
+      <c r="R25" s="14" t="n">
+        <f aca="false">ROUNDUP(C25,0)</f>
+        <v>113785</v>
+      </c>
+      <c r="S25" s="14" t="n">
+        <f aca="false">R25-Q25</f>
+        <v>10360</v>
+      </c>
+      <c r="T25" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q25)+($B$1+$B$5*R25))/2*(R25-Q25)</f>
+        <v>1464852200</v>
+      </c>
+      <c r="U25" s="15" t="n">
+        <f aca="false">T25-$B$7</f>
+        <v>8450</v>
+      </c>
+      <c r="V25" s="9" t="n">
+        <f aca="false">ABS(T25-$B$7)</f>
+        <v>8450</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <f aca="false">$B$7*(A26+1)</f>
+        <v>23437500000</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <f aca="false">-$F$1-SQRT($F$1*$F$1+2*B26/$B$5)</f>
+        <v>125000</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <f aca="false">($B$1+$B$1+$B$5*C26)*C26/2-SUM($D$11:D25)</f>
+        <v>1464843750</v>
+      </c>
+      <c r="E26" s="7" t="n">
+        <f aca="false">F25</f>
+        <v>113784</v>
+      </c>
+      <c r="F26" s="7" t="n">
+        <f aca="false">ROUNDDOWN(C26,0)</f>
+        <v>125000</v>
+      </c>
+      <c r="G26" s="10" t="n">
+        <f aca="false">F26-E26</f>
+        <v>11216</v>
+      </c>
+      <c r="H26" s="11" t="n">
+        <f aca="false">(($B$1+$B$5*E26)+($B$1+$B$5*F26))/2*(F26-E26)</f>
+        <v>1464899328</v>
+      </c>
+      <c r="I26" s="11" t="n">
+        <f aca="false">H26-$B$7</f>
+        <v>55578</v>
+      </c>
+      <c r="J26" s="11" t="n">
+        <f aca="false">ABS(H26-$B$7)</f>
+        <v>55578</v>
+      </c>
+      <c r="K26" s="12" t="n">
+        <f aca="false">L25</f>
+        <v>113784</v>
+      </c>
+      <c r="L26" s="12" t="n">
+        <f aca="false">ROUND(C26,0)</f>
+        <v>125000</v>
+      </c>
+      <c r="M26" s="12" t="n">
+        <f aca="false">L26-K26</f>
+        <v>11216</v>
+      </c>
+      <c r="N26" s="13" t="n">
+        <f aca="false">(($B$1+$B$5*K26)+($B$1+$B$5*L26))/2*(L26-K26)</f>
+        <v>1464899328</v>
+      </c>
+      <c r="O26" s="13" t="n">
+        <f aca="false">N26-$B$7</f>
+        <v>55578</v>
+      </c>
+      <c r="P26" s="13" t="n">
+        <f aca="false">ABS(N26-$B$7)</f>
+        <v>55578</v>
+      </c>
+      <c r="Q26" s="14" t="n">
+        <f aca="false">R25</f>
+        <v>113785</v>
+      </c>
+      <c r="R26" s="14" t="n">
+        <f aca="false">ROUNDUP(C26,0)</f>
+        <v>125000</v>
+      </c>
+      <c r="S26" s="14" t="n">
+        <f aca="false">R26-Q26</f>
+        <v>11215</v>
+      </c>
+      <c r="T26" s="15" t="n">
+        <f aca="false">(($B$1+$B$5*Q26)+($B$1+$B$5*R26))/2*(R26-Q26)</f>
+        <v>1464763112.5</v>
+      </c>
+      <c r="U26" s="15" t="n">
+        <f aca="false">T26-$B$7</f>
+        <v>-80637.5</v>
+      </c>
+      <c r="V26" s="9" t="n">
+        <f aca="false">ABS(T26-$B$7)</f>
+        <v>80637.5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="I28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="17" t="n">
+        <f aca="false">SUM(J11:J26)</f>
+        <v>1204576</v>
+      </c>
+      <c r="O28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28" s="17" t="n">
+        <f aca="false">SUM(P11:P26)</f>
+        <v>1057761</v>
+      </c>
+      <c r="U28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="V28" s="17" t="n">
+        <f aca="false">SUM(V11:V26)</f>
+        <v>1452995</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="19" t="n">
+        <f aca="false">J28</f>
+        <v>1204576</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="19" t="n">
+        <f aca="false">P28</f>
+        <v>1057761</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="19" t="n">
+        <f aca="false">V28</f>
+        <v>1452995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="Q9:V9"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>

</xml_diff>